<commit_message>
Implement hh-based ACF around TB cases detected through PCF
</commit_message>
<xml_diff>
--- a/spreadsheets/common_parameters.xlsx
+++ b/spreadsheets/common_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP-TB\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B68CFD8-25E0-45CF-A9C9-336E15F48F14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30250708-DE7B-43F2-8ED7-51F9BFF2E89D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16400" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="118">
   <si>
     <t>float</t>
   </si>
@@ -377,6 +377,9 @@
   </si>
   <si>
     <t>rate_tb_mortality_closed_tb</t>
+  </si>
+  <si>
+    <t>hh_based_acf_coverage_perc</t>
   </si>
 </sst>
 </file>
@@ -799,32 +802,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="65.7109375" customWidth="1"/>
+    <col min="1" max="1" width="37.7265625" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" customWidth="1"/>
+    <col min="4" max="4" width="65.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="9">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="9"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -838,7 +841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>47</v>
       </c>
@@ -850,7 +853,7 @@
       </c>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>48</v>
       </c>
@@ -862,7 +865,7 @@
       </c>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>49</v>
       </c>
@@ -876,7 +879,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
@@ -888,7 +891,7 @@
       </c>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
@@ -900,7 +903,7 @@
       </c>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
@@ -914,7 +917,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
@@ -928,7 +931,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>95</v>
       </c>
@@ -942,7 +945,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>94</v>
       </c>
@@ -956,7 +959,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
@@ -970,7 +973,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>67</v>
       </c>
@@ -984,7 +987,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>68</v>
       </c>
@@ -998,7 +1001,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="13" t="s">
         <v>71</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
@@ -1026,7 +1029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>106</v>
       </c>
@@ -1038,7 +1041,7 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>107</v>
       </c>
@@ -1052,7 +1055,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>108</v>
       </c>
@@ -1066,7 +1069,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>11</v>
       </c>
@@ -1078,7 +1081,7 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>13</v>
       </c>
@@ -1090,7 +1093,7 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>105</v>
       </c>
@@ -1101,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>100</v>
       </c>
@@ -1112,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>101</v>
       </c>
@@ -1123,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>102</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>103</v>
       </c>
@@ -1148,7 +1151,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>26</v>
       </c>
@@ -1162,7 +1165,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>98</v>
       </c>
@@ -1176,7 +1179,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
@@ -1188,7 +1191,7 @@
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
         <v>28</v>
       </c>
@@ -1200,7 +1203,7 @@
       </c>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
@@ -1214,7 +1217,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
@@ -1228,7 +1231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>78</v>
       </c>
@@ -1242,7 +1245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>5</v>
       </c>
@@ -1254,7 +1257,7 @@
       </c>
       <c r="D34" s="9"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>6</v>
       </c>
@@ -1266,7 +1269,7 @@
       </c>
       <c r="D35" s="9"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>7</v>
       </c>
@@ -1278,7 +1281,7 @@
       </c>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
         <v>8</v>
       </c>
@@ -1290,7 +1293,7 @@
       </c>
       <c r="D37" s="9"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
         <v>9</v>
       </c>
@@ -1302,7 +1305,7 @@
       </c>
       <c r="D38" s="9"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
         <v>10</v>
       </c>
@@ -1314,7 +1317,7 @@
       </c>
       <c r="D39" s="9"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
         <v>88</v>
       </c>
@@ -1328,7 +1331,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
         <v>89</v>
       </c>
@@ -1342,7 +1345,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
         <v>90</v>
       </c>
@@ -1356,7 +1359,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -1368,7 +1371,7 @@
       </c>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>65</v>
       </c>
@@ -1380,7 +1383,7 @@
       </c>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>112</v>
       </c>
@@ -1394,7 +1397,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>113</v>
       </c>
@@ -1408,7 +1411,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>114</v>
       </c>
@@ -1422,7 +1425,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>116</v>
       </c>
@@ -1436,7 +1439,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
         <v>92</v>
       </c>
@@ -1448,7 +1451,7 @@
       </c>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A50" s="12" t="s">
         <v>29</v>
       </c>
@@ -1460,7 +1463,7 @@
       </c>
       <c r="D50" s="12"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>66</v>
       </c>
@@ -1472,7 +1475,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>23</v>
       </c>
@@ -1486,7 +1489,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>24</v>
       </c>
@@ -1500,7 +1503,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>79</v>
       </c>
@@ -1514,7 +1517,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>81</v>
       </c>
@@ -1528,7 +1531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>82</v>
       </c>
@@ -1542,7 +1545,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
         <v>36</v>
       </c>
@@ -1556,7 +1559,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>30</v>
       </c>
@@ -1570,7 +1573,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>39</v>
       </c>
@@ -1582,7 +1585,7 @@
       </c>
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>44</v>
       </c>
@@ -1594,7 +1597,7 @@
       </c>
       <c r="D60" s="5"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>40</v>
       </c>
@@ -1606,7 +1609,7 @@
       </c>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>45</v>
       </c>
@@ -1618,7 +1621,7 @@
       </c>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>33</v>
       </c>
@@ -1630,7 +1633,7 @@
       </c>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>35</v>
       </c>
@@ -1644,7 +1647,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>41</v>
       </c>
@@ -1656,7 +1659,7 @@
       </c>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="6" t="s">
         <v>34</v>
       </c>
@@ -1668,7 +1671,7 @@
       </c>
       <c r="D66" s="6"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
         <v>51</v>
       </c>
@@ -1682,7 +1685,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="6" t="s">
         <v>50</v>
       </c>
@@ -1694,7 +1697,7 @@
       </c>
       <c r="D68" s="6"/>
     </row>
-    <row r="69" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="6" t="s">
         <v>74</v>
       </c>
@@ -1708,7 +1711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="6" t="s">
         <v>75</v>
       </c>
@@ -1722,7 +1725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="6" t="s">
         <v>76</v>
       </c>
@@ -1736,7 +1739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="6" t="s">
         <v>58</v>
       </c>
@@ -1748,7 +1751,7 @@
       </c>
       <c r="D72" s="6"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="6" t="s">
         <v>59</v>
       </c>
@@ -1762,7 +1765,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>84</v>
       </c>
@@ -1776,7 +1779,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>86</v>
       </c>
@@ -1790,7 +1793,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>87</v>
       </c>
@@ -1804,7 +1807,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="16" t="s">
         <v>109</v>
       </c>
@@ -1818,7 +1821,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="16" t="s">
         <v>111</v>
       </c>
@@ -1829,6 +1832,17 @@
         <v>0</v>
       </c>
       <c r="D78" s="16"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1868,9 +1882,9 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1881,7 +1895,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -1892,7 +1906,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1903,7 +1917,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -1911,7 +1925,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Freeze randomness for testing and optimisation
</commit_message>
<xml_diff>
--- a/spreadsheets/common_parameters.xlsx
+++ b/spreadsheets/common_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10112"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP-TB\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msee/Projects/2020/SNAP-TB/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B68CFD8-25E0-45CF-A9C9-336E15F48F14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820A8945-E95E-2544-9F0E-586B4AC5672F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -801,30 +801,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="65.7109375" customWidth="1"/>
+    <col min="1" max="1" width="37.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="65.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="9">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="9"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -838,7 +838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>47</v>
       </c>
@@ -850,7 +850,7 @@
       </c>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>48</v>
       </c>
@@ -862,7 +862,7 @@
       </c>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>49</v>
       </c>
@@ -876,7 +876,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
@@ -888,7 +888,7 @@
       </c>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
@@ -900,7 +900,7 @@
       </c>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
@@ -914,7 +914,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
@@ -928,7 +928,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>95</v>
       </c>
@@ -942,7 +942,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>94</v>
       </c>
@@ -956,7 +956,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
@@ -970,7 +970,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>67</v>
       </c>
@@ -984,7 +984,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>68</v>
       </c>
@@ -998,7 +998,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>71</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>106</v>
       </c>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>107</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>108</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>11</v>
       </c>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>13</v>
       </c>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>105</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>100</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>101</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>102</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>103</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>26</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>98</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
@@ -1188,7 +1188,7 @@
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>28</v>
       </c>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>78</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>5</v>
       </c>
@@ -1254,7 +1254,7 @@
       </c>
       <c r="D34" s="9"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>6</v>
       </c>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="D35" s="9"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>7</v>
       </c>
@@ -1278,7 +1278,7 @@
       </c>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>8</v>
       </c>
@@ -1290,7 +1290,7 @@
       </c>
       <c r="D37" s="9"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>9</v>
       </c>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="D38" s="9"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>10</v>
       </c>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="D39" s="9"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>88</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>89</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>90</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -1368,7 +1368,7 @@
       </c>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>65</v>
       </c>
@@ -1380,7 +1380,7 @@
       </c>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>112</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>113</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>114</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>116</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>92</v>
       </c>
@@ -1448,7 +1448,7 @@
       </c>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="s">
         <v>29</v>
       </c>
@@ -1460,7 +1460,7 @@
       </c>
       <c r="D50" s="12"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>66</v>
       </c>
@@ -1472,7 +1472,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>23</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>24</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>79</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>81</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>82</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>36</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>30</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>39</v>
       </c>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>44</v>
       </c>
@@ -1594,7 +1594,7 @@
       </c>
       <c r="D60" s="5"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>40</v>
       </c>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>45</v>
       </c>
@@ -1618,7 +1618,7 @@
       </c>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>33</v>
       </c>
@@ -1630,7 +1630,7 @@
       </c>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>35</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>41</v>
       </c>
@@ -1656,7 +1656,7 @@
       </c>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>34</v>
       </c>
@@ -1668,7 +1668,7 @@
       </c>
       <c r="D66" s="6"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
         <v>51</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>50</v>
       </c>
@@ -1694,7 +1694,7 @@
       </c>
       <c r="D68" s="6"/>
     </row>
-    <row r="69" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
         <v>74</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
         <v>75</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
         <v>76</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
         <v>58</v>
       </c>
@@ -1748,7 +1748,7 @@
       </c>
       <c r="D72" s="6"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
         <v>59</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>84</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>86</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>87</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="16" t="s">
         <v>109</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="16" t="s">
         <v>111</v>
       </c>
@@ -1868,9 +1868,9 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
update spreadsheets and readme
</commit_message>
<xml_diff>
--- a/spreadsheets/common_parameters.xlsx
+++ b/spreadsheets/common_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20352"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msee/Projects/2020/SNAP-TB/spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP-TB\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820A8945-E95E-2544-9F0E-586B4AC5672F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30250708-DE7B-43F2-8ED7-51F9BFF2E89D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16400" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="118">
   <si>
     <t>float</t>
   </si>
@@ -377,6 +377,9 @@
   </si>
   <si>
     <t>rate_tb_mortality_closed_tb</t>
+  </si>
+  <si>
+    <t>hh_based_acf_coverage_perc</t>
   </si>
 </sst>
 </file>
@@ -799,20 +802,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="65.6640625" customWidth="1"/>
+    <col min="1" max="1" width="37.7265625" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" customWidth="1"/>
+    <col min="4" max="4" width="65.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>46</v>
       </c>
@@ -824,7 +827,7 @@
       </c>
       <c r="D1" s="9"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -838,7 +841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>47</v>
       </c>
@@ -850,7 +853,7 @@
       </c>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>48</v>
       </c>
@@ -862,7 +865,7 @@
       </c>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>49</v>
       </c>
@@ -876,7 +879,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
@@ -888,7 +891,7 @@
       </c>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
@@ -900,7 +903,7 @@
       </c>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
@@ -914,7 +917,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
@@ -928,7 +931,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>95</v>
       </c>
@@ -942,7 +945,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>94</v>
       </c>
@@ -956,7 +959,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
@@ -970,7 +973,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>67</v>
       </c>
@@ -984,7 +987,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>68</v>
       </c>
@@ -998,7 +1001,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="13" t="s">
         <v>71</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
@@ -1026,7 +1029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>106</v>
       </c>
@@ -1038,7 +1041,7 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>107</v>
       </c>
@@ -1052,7 +1055,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>108</v>
       </c>
@@ -1066,7 +1069,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>11</v>
       </c>
@@ -1078,7 +1081,7 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>13</v>
       </c>
@@ -1090,7 +1093,7 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>105</v>
       </c>
@@ -1101,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>100</v>
       </c>
@@ -1112,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>101</v>
       </c>
@@ -1123,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>102</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>103</v>
       </c>
@@ -1148,7 +1151,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>26</v>
       </c>
@@ -1162,7 +1165,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>98</v>
       </c>
@@ -1176,7 +1179,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
@@ -1188,7 +1191,7 @@
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
         <v>28</v>
       </c>
@@ -1200,7 +1203,7 @@
       </c>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
@@ -1214,7 +1217,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
@@ -1228,7 +1231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>78</v>
       </c>
@@ -1242,7 +1245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>5</v>
       </c>
@@ -1254,7 +1257,7 @@
       </c>
       <c r="D34" s="9"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>6</v>
       </c>
@@ -1266,7 +1269,7 @@
       </c>
       <c r="D35" s="9"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>7</v>
       </c>
@@ -1278,7 +1281,7 @@
       </c>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
         <v>8</v>
       </c>
@@ -1290,7 +1293,7 @@
       </c>
       <c r="D37" s="9"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
         <v>9</v>
       </c>
@@ -1302,7 +1305,7 @@
       </c>
       <c r="D38" s="9"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
         <v>10</v>
       </c>
@@ -1314,7 +1317,7 @@
       </c>
       <c r="D39" s="9"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
         <v>88</v>
       </c>
@@ -1328,7 +1331,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
         <v>89</v>
       </c>
@@ -1342,7 +1345,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
         <v>90</v>
       </c>
@@ -1356,7 +1359,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -1368,7 +1371,7 @@
       </c>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>65</v>
       </c>
@@ -1380,7 +1383,7 @@
       </c>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>112</v>
       </c>
@@ -1394,7 +1397,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>113</v>
       </c>
@@ -1408,7 +1411,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>114</v>
       </c>
@@ -1422,7 +1425,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>116</v>
       </c>
@@ -1436,7 +1439,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
         <v>92</v>
       </c>
@@ -1448,7 +1451,7 @@
       </c>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A50" s="12" t="s">
         <v>29</v>
       </c>
@@ -1460,7 +1463,7 @@
       </c>
       <c r="D50" s="12"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>66</v>
       </c>
@@ -1472,7 +1475,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>23</v>
       </c>
@@ -1486,7 +1489,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>24</v>
       </c>
@@ -1500,7 +1503,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>79</v>
       </c>
@@ -1514,7 +1517,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>81</v>
       </c>
@@ -1528,7 +1531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>82</v>
       </c>
@@ -1542,7 +1545,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
         <v>36</v>
       </c>
@@ -1556,7 +1559,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>30</v>
       </c>
@@ -1570,7 +1573,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>39</v>
       </c>
@@ -1582,7 +1585,7 @@
       </c>
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>44</v>
       </c>
@@ -1594,7 +1597,7 @@
       </c>
       <c r="D60" s="5"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>40</v>
       </c>
@@ -1606,7 +1609,7 @@
       </c>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>45</v>
       </c>
@@ -1618,7 +1621,7 @@
       </c>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>33</v>
       </c>
@@ -1630,7 +1633,7 @@
       </c>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>35</v>
       </c>
@@ -1644,7 +1647,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>41</v>
       </c>
@@ -1656,7 +1659,7 @@
       </c>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="6" t="s">
         <v>34</v>
       </c>
@@ -1668,7 +1671,7 @@
       </c>
       <c r="D66" s="6"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
         <v>51</v>
       </c>
@@ -1682,7 +1685,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="6" t="s">
         <v>50</v>
       </c>
@@ -1694,7 +1697,7 @@
       </c>
       <c r="D68" s="6"/>
     </row>
-    <row r="69" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="6" t="s">
         <v>74</v>
       </c>
@@ -1708,7 +1711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="6" t="s">
         <v>75</v>
       </c>
@@ -1722,7 +1725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="6" t="s">
         <v>76</v>
       </c>
@@ -1736,7 +1739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="6" t="s">
         <v>58</v>
       </c>
@@ -1748,7 +1751,7 @@
       </c>
       <c r="D72" s="6"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="6" t="s">
         <v>59</v>
       </c>
@@ -1762,7 +1765,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>84</v>
       </c>
@@ -1776,7 +1779,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>86</v>
       </c>
@@ -1790,7 +1793,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>87</v>
       </c>
@@ -1804,7 +1807,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="16" t="s">
         <v>109</v>
       </c>
@@ -1818,7 +1821,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="16" t="s">
         <v>111</v>
       </c>
@@ -1829,6 +1832,17 @@
         <v>0</v>
       </c>
       <c r="D78" s="16"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1868,9 +1882,9 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1881,7 +1895,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -1892,7 +1906,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1903,7 +1917,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -1911,7 +1925,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Optimisation of various parts Also up size of simulation
</commit_message>
<xml_diff>
--- a/spreadsheets/common_parameters.xlsx
+++ b/spreadsheets/common_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10112"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP-TB\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msee/Projects/2020/SNAP-TB/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30250708-DE7B-43F2-8ED7-51F9BFF2E89D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCA8163-0F42-0845-9867-220B590DFCE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16400" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -804,30 +804,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.7265625" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" customWidth="1"/>
-    <col min="4" max="4" width="65.7265625" customWidth="1"/>
+    <col min="1" max="1" width="37.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="65.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="9">
-        <v>10000</v>
+        <v>40000</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="9"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -841,7 +841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>47</v>
       </c>
@@ -853,7 +853,7 @@
       </c>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>48</v>
       </c>
@@ -865,7 +865,7 @@
       </c>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>49</v>
       </c>
@@ -879,7 +879,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
@@ -891,7 +891,7 @@
       </c>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
@@ -903,7 +903,7 @@
       </c>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
@@ -917,7 +917,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
@@ -931,7 +931,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>95</v>
       </c>
@@ -945,7 +945,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>94</v>
       </c>
@@ -959,7 +959,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
@@ -973,7 +973,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>67</v>
       </c>
@@ -987,7 +987,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>68</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>71</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>106</v>
       </c>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>107</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>108</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>11</v>
       </c>
@@ -1081,7 +1081,7 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>13</v>
       </c>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>105</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>100</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>101</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>102</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>103</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>26</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>98</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>28</v>
       </c>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>78</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>5</v>
       </c>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="D34" s="9"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>6</v>
       </c>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="D35" s="9"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>7</v>
       </c>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>8</v>
       </c>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="D37" s="9"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>9</v>
       </c>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="D38" s="9"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>10</v>
       </c>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="D39" s="9"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>88</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>89</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>90</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>65</v>
       </c>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>112</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>113</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>114</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>116</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>92</v>
       </c>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="s">
         <v>29</v>
       </c>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="D50" s="12"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>66</v>
       </c>
@@ -1475,7 +1475,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>23</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>24</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>79</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>81</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>82</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>36</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>30</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>39</v>
       </c>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>44</v>
       </c>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="D60" s="5"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>40</v>
       </c>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>45</v>
       </c>
@@ -1621,7 +1621,7 @@
       </c>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>33</v>
       </c>
@@ -1633,7 +1633,7 @@
       </c>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>35</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>41</v>
       </c>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>34</v>
       </c>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="D66" s="6"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
         <v>51</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>50</v>
       </c>
@@ -1697,7 +1697,7 @@
       </c>
       <c r="D68" s="6"/>
     </row>
-    <row r="69" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
         <v>74</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
         <v>75</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
         <v>76</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
         <v>58</v>
       </c>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="D72" s="6"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
         <v>59</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>84</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>86</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>87</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="16" t="s">
         <v>109</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="16" t="s">
         <v>111</v>
       </c>
@@ -1833,7 +1833,7 @@
       </c>
       <c r="D78" s="16"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>117</v>
       </c>
@@ -1882,9 +1882,9 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Add spreadsheets for full run
</commit_message>
<xml_diff>
--- a/spreadsheets/common_parameters.xlsx
+++ b/spreadsheets/common_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20352"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msee/Projects/2020/SNAP-TB/spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.monash.edu\home\User048\rrag0004\Desktop\config_snap_tb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCA8163-0F42-0845-9867-220B590DFCE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB839399-E5FB-415A-A01C-613FD03F9D82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -804,30 +804,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="65.6640625" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="65.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="9">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="9"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -841,7 +841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>47</v>
       </c>
@@ -853,7 +853,7 @@
       </c>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>48</v>
       </c>
@@ -865,7 +865,7 @@
       </c>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>49</v>
       </c>
@@ -879,7 +879,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
@@ -891,7 +891,7 @@
       </c>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
@@ -903,7 +903,7 @@
       </c>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
@@ -917,7 +917,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
@@ -931,7 +931,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>95</v>
       </c>
@@ -945,7 +945,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>94</v>
       </c>
@@ -959,7 +959,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
@@ -973,7 +973,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>67</v>
       </c>
@@ -987,7 +987,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>68</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>71</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>106</v>
       </c>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>107</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>108</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>11</v>
       </c>
@@ -1081,7 +1081,7 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>13</v>
       </c>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>105</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>100</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>101</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>102</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>103</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>26</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>98</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>28</v>
       </c>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>78</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>5</v>
       </c>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="D34" s="9"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>6</v>
       </c>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="D35" s="9"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>7</v>
       </c>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>8</v>
       </c>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="D37" s="9"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>9</v>
       </c>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="D38" s="9"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>10</v>
       </c>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="D39" s="9"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>88</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>89</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>90</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>65</v>
       </c>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>112</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>113</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>114</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>116</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>92</v>
       </c>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>29</v>
       </c>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="D50" s="12"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>66</v>
       </c>
@@ -1475,7 +1475,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>23</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>24</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>79</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>81</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>82</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>36</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>30</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>39</v>
       </c>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>44</v>
       </c>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="D60" s="5"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>40</v>
       </c>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>45</v>
       </c>
@@ -1621,7 +1621,7 @@
       </c>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>33</v>
       </c>
@@ -1633,7 +1633,7 @@
       </c>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>35</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>41</v>
       </c>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>34</v>
       </c>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="D66" s="6"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>51</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>50</v>
       </c>
@@ -1697,7 +1697,7 @@
       </c>
       <c r="D68" s="6"/>
     </row>
-    <row r="69" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>74</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>75</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>76</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>58</v>
       </c>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="D72" s="6"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>59</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>84</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>86</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>87</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
         <v>109</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
         <v>111</v>
       </c>
@@ -1833,7 +1833,7 @@
       </c>
       <c r="D78" s="16"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>117</v>
       </c>
@@ -1882,9 +1882,9 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Begin add disease class tests Begin testing model step
cleanup gitignore
</commit_message>
<xml_diff>
--- a/spreadsheets/common_parameters.xlsx
+++ b/spreadsheets/common_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.monash.edu\home\User048\rrag0004\Desktop\config_snap_tb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msee/Projects/2020/SNAP-TB/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB839399-E5FB-415A-A01C-613FD03F9D82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C18FE0-C707-0343-AD4A-139B2F738CE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -805,17 +805,17 @@
   <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="65.7109375" customWidth="1"/>
+    <col min="1" max="1" width="37.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="65.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>46</v>
       </c>
@@ -827,7 +827,7 @@
       </c>
       <c r="D1" s="9"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -841,7 +841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>47</v>
       </c>
@@ -853,7 +853,7 @@
       </c>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>48</v>
       </c>
@@ -865,7 +865,7 @@
       </c>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>49</v>
       </c>
@@ -879,7 +879,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
@@ -891,7 +891,7 @@
       </c>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
@@ -903,7 +903,7 @@
       </c>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
@@ -917,7 +917,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
@@ -931,7 +931,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>95</v>
       </c>
@@ -945,7 +945,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>94</v>
       </c>
@@ -959,7 +959,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
@@ -973,7 +973,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>67</v>
       </c>
@@ -987,7 +987,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>68</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>71</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>106</v>
       </c>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>107</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>108</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>11</v>
       </c>
@@ -1081,7 +1081,7 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>13</v>
       </c>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>105</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>100</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>101</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>102</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>103</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>26</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>98</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>28</v>
       </c>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>78</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>5</v>
       </c>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="D34" s="9"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>6</v>
       </c>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="D35" s="9"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>7</v>
       </c>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>8</v>
       </c>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="D37" s="9"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>9</v>
       </c>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="D38" s="9"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>10</v>
       </c>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="D39" s="9"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>88</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>89</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>90</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>65</v>
       </c>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>112</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>113</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>114</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>116</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>92</v>
       </c>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="s">
         <v>29</v>
       </c>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="D50" s="12"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>66</v>
       </c>
@@ -1475,7 +1475,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>23</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>24</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>79</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>81</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>82</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>36</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>30</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>39</v>
       </c>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>44</v>
       </c>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="D60" s="5"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>40</v>
       </c>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>45</v>
       </c>
@@ -1621,7 +1621,7 @@
       </c>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>33</v>
       </c>
@@ -1633,7 +1633,7 @@
       </c>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>35</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>41</v>
       </c>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>34</v>
       </c>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="D66" s="6"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
         <v>51</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>50</v>
       </c>
@@ -1697,7 +1697,7 @@
       </c>
       <c r="D68" s="6"/>
     </row>
-    <row r="69" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
         <v>74</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
         <v>75</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
         <v>76</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
         <v>58</v>
       </c>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="D72" s="6"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
         <v>59</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>84</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>86</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>87</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="16" t="s">
         <v>109</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="16" t="s">
         <v>111</v>
       </c>
@@ -1833,7 +1833,7 @@
       </c>
       <c r="D78" s="16"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>117</v>
       </c>
@@ -1849,7 +1849,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>dropdown!$C$1:$C$3</xm:f>
@@ -1882,9 +1882,9 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>73</v>
       </c>

</xml_diff>